<commit_message>
Improve table of contents for all forms
</commit_message>
<xml_diff>
--- a/odkx/app/config/tables/hh_geo_location/forms/hh_geo_location/hh_geo_location.xlsx
+++ b/odkx/app/config/tables/hh_geo_location/forms/hh_geo_location/hh_geo_location.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="61">
   <si>
     <t xml:space="preserve">clause</t>
   </si>
@@ -103,9 +103,6 @@
   </si>
   <si>
     <t xml:space="preserve">survey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Geo Location</t>
   </si>
   <si>
     <t xml:space="preserve">Household Geolocation</t>
@@ -407,7 +404,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -452,7 +449,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16"/>
@@ -509,231 +506,134 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R9"/>
+  <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L9" activeCellId="0" sqref="L9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="16.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="19.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.37"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.13"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="12.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="19.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="20.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="20.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="19.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="20.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1015" style="0" width="11.12"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="L1" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="O1" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="P1" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="R1" s="0" t="s">
-        <v>21</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="0" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>20210221001</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>20210204001</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>20210221001</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="L4" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="0" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="0" t="s">
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="N5" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="0" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="F6" s="0" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K6" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="P6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q6" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="R6" s="0" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
+      <c r="F7" s="0" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="R7" s="0" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="F8" s="0" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q8" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="R8" s="0" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K9" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="0" t="n">
+      <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
     </row>
@@ -759,7 +659,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="14"/>
@@ -769,13 +669,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>37</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
@@ -786,87 +686,87 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -891,7 +791,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.3"/>
   </cols>
@@ -906,10 +806,10 @@
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -942,7 +842,7 @@
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.21875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.49"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="37.56"/>
@@ -950,16 +850,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="C1" s="0" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="D1" s="0" t="s">
         <v>54</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,13 +867,13 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>56</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,13 +881,13 @@
         <v>13</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>59</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>60</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>